<commit_message>
Update Silent Space Audio Asset List.xlsx
</commit_message>
<xml_diff>
--- a/Silent Space Audio Asset List.xlsx
+++ b/Silent Space Audio Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wmii/Documents/GitHub/MetroidvaniaHorrorGame/Metroidvania Horror Unity Project Settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429ACCEB-1AAA-7841-8511-9D56361E9F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE695521-40B6-8B4D-A960-8E8FDAE57E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52600" yWindow="7700" windowWidth="38520" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1517,8 +1517,8 @@
   </sheetPr>
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2987,7 +2987,7 @@
       <c r="B66">
         <v>63</v>
       </c>
-      <c r="C66" s="10"/>
+      <c r="C66" s="15"/>
       <c r="D66" t="s">
         <v>239</v>
       </c>

</xml_diff>